<commit_message>
Finish Paper and Code
YAYYY!!!!!!

It's important to note a fair amount of code is different than what appears in my final paper. I hope to go back and fix mistakes later.
</commit_message>
<xml_diff>
--- a/social_research/APA tables.xlsx
+++ b/social_research/APA tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byrds\Documents\rStudio_work\social_research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580C1FB7-C966-4442-8588-BE7F7429A44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87115ED8-F72F-4E17-9B8F-8A3B0FAF3566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{881C638E-C4B8-4850-BFF4-3DD1988B90C8}"/>
+    <workbookView xWindow="90" yWindow="0" windowWidth="12970" windowHeight="12090" xr2:uid="{881C638E-C4B8-4850-BFF4-3DD1988B90C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>df</t>
   </si>
@@ -86,15 +86,9 @@
     <t>Estimate</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>Non-Parametric Test</t>
   </si>
   <si>
-    <t>Race/Ethnicity</t>
-  </si>
-  <si>
     <t>None|GED</t>
   </si>
   <si>
@@ -131,17 +125,56 @@
     <t>Pr(&gt;|t|)</t>
   </si>
   <si>
-    <t>Intercept</t>
-  </si>
-  <si>
     <t>Coefficients</t>
+  </si>
+  <si>
+    <t>Mixed Race*</t>
+  </si>
+  <si>
+    <t>HGC Mom:Black</t>
+  </si>
+  <si>
+    <t>HGC Mom:Hispanic</t>
+  </si>
+  <si>
+    <t>HGC Mom:Mixed</t>
+  </si>
+  <si>
+    <t>Black:HGC Dad</t>
+  </si>
+  <si>
+    <t>Hispanic:HGC Dad</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Mixed:HGC Dad</t>
+  </si>
+  <si>
+    <t>(Intercept)</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>f-Stat</t>
+  </si>
+  <si>
+    <t>Utilizes svyglm before I fixed svyolr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +192,19 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -242,26 +288,50 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -600,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAA8B3F-B5D5-42B9-97C9-640E21A96EE3}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -611,15 +681,17 @@
     <col min="1" max="1" width="13.7265625" customWidth="1"/>
     <col min="2" max="2" width="13.453125" customWidth="1"/>
     <col min="3" max="4" width="18.36328125" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" customWidth="1"/>
+    <col min="9" max="9" width="16.26953125" customWidth="1"/>
     <col min="10" max="12" width="9.7265625" customWidth="1"/>
     <col min="13" max="13" width="9.36328125" customWidth="1"/>
-    <col min="16" max="16" width="12.81640625" customWidth="1"/>
-    <col min="17" max="20" width="9.6328125" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
+    <col min="16" max="16" width="9.90625" customWidth="1"/>
+    <col min="17" max="17" width="16.54296875" customWidth="1"/>
+    <col min="18" max="20" width="9.6328125" customWidth="1"/>
     <col min="22" max="22" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -634,13 +706,17 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="Q1" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -662,8 +738,10 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -671,44 +749,36 @@
       <c r="E3" s="2"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="8" t="s">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" s="6"/>
-      <c r="P3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="T3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="U3" s="2"/>
-    </row>
-    <row r="4" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="U3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="V3" s="2"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+    </row>
+    <row r="4" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -716,86 +786,98 @@
       <c r="E4" s="2"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="16" t="s">
+      <c r="H4" s="2"/>
+      <c r="I4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="6"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0.278254</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0.13480900000000001</v>
+      </c>
+      <c r="T4" s="2">
+        <v>2.0640000000000001</v>
+      </c>
+      <c r="U4" s="17">
+        <v>3.9051000000000002E-2</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="B5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="23"/>
+      <c r="F5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0.59137899999999999</v>
-      </c>
-      <c r="R4" s="2">
-        <v>8.2831000000000002E-2</v>
-      </c>
-      <c r="S4" s="2">
-        <v>7.14</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="U4" s="2"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.1129312</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1.120928E-2</v>
-      </c>
-      <c r="L5" s="2">
-        <v>10.074795999999999</v>
-      </c>
-      <c r="M5" s="2">
-        <v>147.94229999999999</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>8.8172E-2</v>
-      </c>
       <c r="R5" s="2">
-        <v>8.3379999999999999E-3</v>
+        <v>0.117171</v>
       </c>
       <c r="S5" s="2">
-        <v>10.574</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="U5" s="2"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+        <v>1.1554E-2</v>
+      </c>
+      <c r="T5" s="2">
+        <v>10.141</v>
+      </c>
+      <c r="U5" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -807,44 +889,48 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.14384659999999999</v>
-      </c>
-      <c r="K6" s="2">
-        <v>1.8648270000000002E-2</v>
-      </c>
-      <c r="L6" s="2">
-        <v>14.276589</v>
-      </c>
-      <c r="M6" s="2">
-        <v>146.94290000000001</v>
-      </c>
-      <c r="N6" s="11" t="s">
+      <c r="H6" s="12"/>
+      <c r="I6" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="17">
+        <v>0.163163263</v>
+      </c>
+      <c r="K6" s="17">
+        <v>1.8014160000000001E-2</v>
+      </c>
+      <c r="L6" s="17">
+        <v>9.0575029300000001</v>
+      </c>
+      <c r="M6" s="17">
+        <v>56.984969999999997</v>
+      </c>
+      <c r="N6" s="18" t="s">
         <v>2</v>
       </c>
       <c r="O6" s="6"/>
-      <c r="P6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0.121326</v>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="R6" s="2">
-        <v>6.96E-3</v>
+        <v>0.12532799999999999</v>
       </c>
       <c r="S6" s="2">
-        <v>17.431999999999999</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="U6" s="2"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+        <v>0.252801</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0.496</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0.62008200000000002</v>
+      </c>
+      <c r="V6" s="2"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
       <c r="B7" s="2">
         <v>1</v>
@@ -862,44 +948,50 @@
         <v>3917</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="J7" s="2">
-        <v>0.1602952</v>
+        <v>-0.28874248000000002</v>
       </c>
       <c r="K7" s="2">
-        <v>1.8648270000000002E-2</v>
+        <v>0.41608864000000001</v>
       </c>
       <c r="L7" s="2">
-        <v>8.5957139999999992</v>
+        <v>-0.69394462999999995</v>
       </c>
       <c r="M7" s="2">
-        <v>520.23389999999995</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>2</v>
+        <v>33.101759999999999</v>
+      </c>
+      <c r="N7" s="13">
+        <v>0.49255850000000001</v>
       </c>
       <c r="O7" s="6"/>
-      <c r="P7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>9.4713000000000006E-2</v>
-      </c>
-      <c r="R7" s="4">
-        <v>1.3034E-2</v>
-      </c>
-      <c r="S7" s="4">
-        <v>7.2670000000000003</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="U7" s="2"/>
-    </row>
-    <row r="8" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P7" s="2"/>
+      <c r="Q7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1.764051</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0.174008</v>
+      </c>
+      <c r="T7" s="2">
+        <v>10.138</v>
+      </c>
+      <c r="U7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+    </row>
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="2">
         <v>2</v>
@@ -917,16 +1009,48 @@
         <v>1968</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="2">
+        <v>2.6211007450000001</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.26967007999999998</v>
+      </c>
+      <c r="L8" s="17">
+        <v>9.7196572999999997</v>
+      </c>
+      <c r="M8" s="2">
+        <v>185.77305999999999</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>2</v>
+      </c>
       <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R8" s="2">
+        <v>-0.275646</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.92262900000000003</v>
+      </c>
+      <c r="T8" s="2">
+        <v>-0.29899999999999999</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0.76513200000000003</v>
+      </c>
+      <c r="V8" s="2"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="2">
         <v>3</v>
@@ -944,16 +1068,50 @@
         <v>456</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="2">
+        <v>-0.33978609999999998</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1.4578295999999999</v>
+      </c>
+      <c r="L9" s="2">
+        <v>-0.23307669</v>
+      </c>
+      <c r="M9" s="2">
+        <v>975.11494000000005</v>
+      </c>
+      <c r="N9" s="13">
+        <v>0.8157508</v>
+      </c>
       <c r="O9" s="6"/>
       <c r="P9" s="2"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="Q9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0.142678</v>
+      </c>
+      <c r="S9" s="2">
+        <v>9.5530000000000007E-3</v>
+      </c>
+      <c r="T9" s="2">
+        <v>14.935</v>
+      </c>
+      <c r="U9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="4">
         <v>4</v>
@@ -971,24 +1129,48 @@
         <v>262</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="16" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
+      <c r="J10" s="2">
+        <v>0.204763853</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1.4642199999999999E-2</v>
+      </c>
+      <c r="L10" s="17">
+        <v>13.984500690000001</v>
+      </c>
+      <c r="M10" s="2">
+        <v>144.98008999999999</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>2</v>
+      </c>
       <c r="O10" s="6"/>
       <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="Q10" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="R10" s="2">
+        <v>2.8285999999999999E-2</v>
+      </c>
+      <c r="S10" s="2">
+        <v>2.2245999999999998E-2</v>
+      </c>
+      <c r="T10" s="2">
+        <v>1.272</v>
+      </c>
+      <c r="U10" s="2">
+        <v>0.203593</v>
+      </c>
+      <c r="V10" s="2"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
       <c r="B11" s="7" t="s">
         <v>10</v>
@@ -1002,42 +1184,58 @@
         <v>2</v>
       </c>
       <c r="E11" s="8">
-        <f t="shared" ref="E11:F11" si="0">SUM(E7:E10)</f>
+        <f>SUM(E7:E10)</f>
         <v>2</v>
       </c>
       <c r="F11" s="8">
-        <f t="shared" si="0"/>
+        <f>SUM(F7:F10)</f>
         <v>6603</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="2" t="s">
-        <v>19</v>
+      <c r="H11" s="2"/>
+      <c r="I11" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="J11" s="2">
-        <v>0.92265790000000003</v>
+        <v>4.2615127000000003E-2</v>
       </c>
       <c r="K11" s="2">
-        <v>0.11554605</v>
+        <v>3.1517829999999997E-2</v>
       </c>
       <c r="L11" s="2">
-        <v>7.9851960000000002</v>
+        <v>1.3520958700000001</v>
       </c>
       <c r="M11" s="2">
-        <v>1258.2746999999999</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>2</v>
+        <v>85.627139999999997</v>
+      </c>
+      <c r="N11" s="13">
+        <v>0.17990510000000001</v>
       </c>
       <c r="O11" s="6"/>
       <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="Q11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11" s="2">
+        <v>-7.0874000000000006E-2</v>
+      </c>
+      <c r="S11" s="2">
+        <v>1.8047000000000001E-2</v>
+      </c>
+      <c r="T11" s="2">
+        <v>-3.927</v>
+      </c>
+      <c r="U11" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1045,158 +1243,252 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="2" t="s">
-        <v>20</v>
+      <c r="H12" s="2"/>
+      <c r="I12" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="J12" s="2">
-        <v>2.1366787</v>
+        <v>-0.113791768</v>
       </c>
       <c r="K12" s="2">
-        <v>0.11384089</v>
-      </c>
-      <c r="L12" s="2">
-        <v>18.768992000000001</v>
+        <v>2.8842059999999999E-2</v>
+      </c>
+      <c r="L12" s="17">
+        <v>-3.9453412299999999</v>
       </c>
       <c r="M12" s="2">
-        <v>860.96469999999999</v>
-      </c>
-      <c r="N12" s="2" t="s">
+        <v>42.096710000000002</v>
+      </c>
+      <c r="N12" s="17" t="s">
         <v>2</v>
       </c>
       <c r="O12" s="6"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R12" s="2">
+        <v>2.0632999999999999E-2</v>
+      </c>
+      <c r="S12" s="2">
+        <v>6.8753999999999996E-2</v>
+      </c>
+      <c r="T12" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="U12" s="2">
+        <v>0.76410800000000001</v>
+      </c>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="2" t="s">
-        <v>21</v>
+      <c r="H13" s="2"/>
+      <c r="I13" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="J13" s="2">
-        <v>4.1726089999999996</v>
+        <v>-3.684334E-3</v>
       </c>
       <c r="K13" s="2">
-        <v>0.12280189</v>
+        <v>0.11898905999999999</v>
       </c>
       <c r="L13" s="2">
-        <v>33.978377999999999</v>
+        <v>-3.0963629999999999E-2</v>
       </c>
       <c r="M13" s="2">
-        <v>696.83230000000003</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>2</v>
+        <v>91.327340000000007</v>
+      </c>
+      <c r="N13" s="13">
+        <v>0.97536610000000001</v>
       </c>
       <c r="O13" s="6"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="P13" s="2"/>
+      <c r="Q13" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="R13" s="2">
+        <v>-6.4504000000000006E-2</v>
+      </c>
+      <c r="S13" s="2">
+        <v>1.6948999999999999E-2</v>
+      </c>
+      <c r="T13" s="2">
+        <v>-3.806</v>
+      </c>
+      <c r="U13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
       <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="J14" s="2">
-        <v>4.6396841999999996</v>
+        <v>-5.9038476999999999E-2</v>
       </c>
       <c r="K14" s="2">
-        <v>0.12554164000000001</v>
+        <v>3.7133470000000002E-2</v>
       </c>
       <c r="L14" s="2">
-        <v>36.957332000000001</v>
+        <v>-1.58989906</v>
       </c>
       <c r="M14" s="2">
-        <v>676.3646</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>2</v>
+        <v>10.50609</v>
+      </c>
+      <c r="N14" s="13">
+        <v>0.14471600000000001</v>
       </c>
       <c r="O14" s="6"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="P14" s="2"/>
+      <c r="Q14" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="R14" s="2">
+        <v>-7.8902E-2</v>
+      </c>
+      <c r="S14" s="2">
+        <v>1.5649E-2</v>
+      </c>
+      <c r="T14" s="2">
+        <v>-5.0419999999999998</v>
+      </c>
+      <c r="U14" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="V14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" s="6"/>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
+      <c r="C15" s="24"/>
+      <c r="D15" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="2" t="s">
-        <v>23</v>
+      <c r="H15" s="2"/>
+      <c r="I15" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="J15" s="2">
-        <v>6.2373972999999996</v>
+        <v>-0.11022069900000001</v>
       </c>
       <c r="K15" s="2">
-        <v>0.1362459</v>
-      </c>
-      <c r="L15" s="2">
-        <v>45.780441000000003</v>
+        <v>2.6111019999999999E-2</v>
+      </c>
+      <c r="L15" s="17">
+        <v>-4.2212324499999996</v>
       </c>
       <c r="M15" s="2">
-        <v>727.29759999999999</v>
-      </c>
-      <c r="N15" s="2" t="s">
+        <v>41.145780000000002</v>
+      </c>
+      <c r="N15" s="17" t="s">
         <v>2</v>
       </c>
       <c r="O15" s="6"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="P15" s="2"/>
+      <c r="Q15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R15" s="4">
+        <v>-2.9156000000000001E-2</v>
+      </c>
+      <c r="S15" s="4">
+        <v>5.3379000000000003E-2</v>
+      </c>
+      <c r="T15" s="4">
+        <v>-0.54600000000000004</v>
+      </c>
+      <c r="U15" s="4">
+        <v>0.58493499999999998</v>
+      </c>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
-      <c r="B16" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="B16" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16" s="4">
-        <v>8.8384867000000007</v>
-      </c>
-      <c r="K16" s="4">
-        <v>0.19316238999999999</v>
-      </c>
-      <c r="L16" s="4">
-        <v>45.756767000000004</v>
-      </c>
-      <c r="M16" s="4">
-        <v>1944.3151</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>2</v>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="2">
+        <v>-1.4649419E-2</v>
+      </c>
+      <c r="K16" s="2">
+        <v>9.8616750000000003E-2</v>
+      </c>
+      <c r="L16" s="2">
+        <v>-0.14854899999999999</v>
+      </c>
+      <c r="M16" s="2">
+        <v>456.73908999999998</v>
+      </c>
+      <c r="N16" s="13">
+        <v>0.88197510000000001</v>
       </c>
       <c r="O16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1204,8 +1496,28 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17" s="2"/>
+      <c r="I17" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1213,8 +1525,36 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="1">
+        <v>-0.78574601099999997</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.20629012999999999</v>
+      </c>
+      <c r="L18" s="1">
+        <v>8.6564781199999992</v>
+      </c>
+      <c r="M18" s="1">
+        <v>313.04766000000001</v>
+      </c>
+      <c r="N18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1222,14 +1562,176 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="1">
+        <v>3.0015602480000001</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.20380751999999999</v>
+      </c>
+      <c r="L19" s="1">
+        <v>14.727426100000001</v>
+      </c>
+      <c r="M19" s="1">
+        <v>321.19004999999999</v>
+      </c>
+      <c r="N19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="G20" s="6"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="1">
+        <v>5.056020137</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.20867604000000001</v>
+      </c>
+      <c r="L20" s="1">
+        <v>24.229039660000002</v>
+      </c>
+      <c r="M20" s="1">
+        <v>313.74435999999997</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="G21" s="6"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="1">
+        <v>5.5361056580000003</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.21087602999999999</v>
+      </c>
+      <c r="L21" s="1">
+        <v>26.252891609999999</v>
+      </c>
+      <c r="M21" s="1">
+        <v>320.14326999999997</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="G22" s="6"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="1">
+        <v>7.1869071419999999</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.22091155000000001</v>
+      </c>
+      <c r="L22" s="1">
+        <v>32.532962580000003</v>
+      </c>
+      <c r="M22" s="1">
+        <v>378.22444000000002</v>
+      </c>
+      <c r="N22" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="G23" s="6"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="15">
+        <v>9.8210439209999993</v>
+      </c>
+      <c r="K23" s="15">
+        <v>0.26226588000000001</v>
+      </c>
+      <c r="L23" s="15">
+        <v>37.446899029999997</v>
+      </c>
+      <c r="M23" s="15">
+        <v>724.34889999999996</v>
+      </c>
+      <c r="N23" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="G24" s="6"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="I5:N5"/>
+    <mergeCell ref="I17:N17"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="I10:N10"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B15:C15"/>

</xml_diff>